<commit_message>
Split pricing and uw
</commit_message>
<xml_diff>
--- a/automation/Repository/Pricing.xlsx
+++ b/automation/Repository/Pricing.xlsx
@@ -13,10 +13,11 @@
   </bookViews>
   <sheets>
     <sheet name="TC_05_06" sheetId="5" r:id="rId1"/>
-    <sheet name="Error" sheetId="2" r:id="rId2"/>
-    <sheet name="Contract" sheetId="1" r:id="rId3"/>
-    <sheet name="Calculate" sheetId="4" r:id="rId4"/>
-    <sheet name="OverRide" sheetId="3" r:id="rId5"/>
+    <sheet name="TC16_17" sheetId="6" r:id="rId2"/>
+    <sheet name="Error" sheetId="2" r:id="rId3"/>
+    <sheet name="Contract" sheetId="1" r:id="rId4"/>
+    <sheet name="Calculate" sheetId="4" r:id="rId5"/>
+    <sheet name="OverRide" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="61">
   <si>
     <t>processed</t>
   </si>
@@ -206,6 +207,45 @@
   </si>
   <si>
     <t>SNF</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Coverage_Type</t>
+  </si>
+  <si>
+    <t>Mileage_Band</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Surcharge</t>
+  </si>
+  <si>
+    <t>Option</t>
+  </si>
+  <si>
+    <t>Deductibles</t>
+  </si>
+  <si>
+    <t>SNE</t>
+  </si>
+  <si>
+    <t>Powertrain</t>
+  </si>
+  <si>
+    <t>0-60</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>24/24</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -547,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -727,6 +767,113 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="14.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="9" max="9" width="11.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -768,7 +915,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -812,7 +959,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -856,7 +1003,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>